<commit_message>
Making RTM file but it need more work.
</commit_message>
<xml_diff>
--- a/Software Specifications/Traceability/RTM.xlsx
+++ b/Software Specifications/Traceability/RTM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -13,9 +13,35 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>CRS</t>
+  </si>
+  <si>
+    <t>CYRS</t>
+  </si>
+  <si>
+    <t>SRS or HIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At startup, WELCOME mode shall be one of the following modes:
+● First mode: LEDs shall be ON from L6 to L1, then from R1 to R6 and vice versa, and then all LEDs are ON and OFF.
+● Second mode: LEDS from R1 to R6 are ON LED by LED and also the left branch at the same time, and then repeat the scenario again.
+</t>
+  </si>
+  <si>
+    <t>Tail function shall be activated according to Tail switch.</t>
+  </si>
+  <si>
+    <t>TI function shall be activated be activated according to TI switch, LEDs shall be activated LED by LED from R1 to R6 or from L1 to L6.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -24,15 +50,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -40,18 +72,165 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +277,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +312,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +520,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="116.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+    </row>
+    <row r="4" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>